<commit_message>
Implemented functionality so that usernames are not duplicated upon registration
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -407,60 +407,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented login functionality? Not sure if it is correct, the rest is going to have to be done with the device itself, this is a login into a portal, not a device, maybe this will work?
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -383,27 +383,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>Uday</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>Sharma</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>sharmauday1999@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>uday</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>uday</t>
         </is>
       </c>
     </row>

</xml_diff>